<commit_message>
Atualização do DER - Adição do campo CEP
</commit_message>
<xml_diff>
--- a/Excel/IdeiaCSV.csv.xlsx
+++ b/Excel/IdeiaCSV.csv.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Área de Trabalho\BandTec\3º Semestre\Repositórios\Documentacao-AUTG\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CCE771-88C4-4B23-AD96-0CD4C3B4D65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B4F70-94D2-4F2F-B309-8C0527E2B06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A3205BFF-4DEB-4AA1-82FB-85670DF32728}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório Detalhado" sheetId="1" r:id="rId1"/>
-    <sheet name="Relatório Simples" sheetId="3" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Prédio</t>
   </si>
@@ -366,9 +365,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -410,6 +406,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1799,7 +1798,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1811,13 +1810,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -1827,7 +1826,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1845,22 +1844,22 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="7"/>
@@ -1887,28 +1886,28 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1937,28 +1936,28 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1969,7 +1968,7 @@
       <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="25">
         <v>150696</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1986,7 +1985,7 @@
       <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="25">
         <v>150696</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -2003,7 +2002,7 @@
       <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="25">
         <v>150696</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -2020,7 +2019,7 @@
       <c r="B18" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="25">
         <v>150696</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -2037,7 +2036,7 @@
       <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="25">
         <v>150696</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2054,7 +2053,7 @@
       <c r="B20" s="4">
         <v>1</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="25">
         <v>150696</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -2071,7 +2070,7 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="25">
         <v>150696</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -2088,7 +2087,7 @@
       <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="25">
         <v>150696</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -2106,7 +2105,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -2117,10 +2116,10 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <f>SUM(C15:C22)</f>
         <v>1205568</v>
       </c>
@@ -2129,10 +2128,10 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="15">
         <f>SUM(E15:E22)</f>
         <v>346.48</v>
       </c>
@@ -2156,186 +2155,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4D9E34-09D1-4386-AA71-D54C2FF510C9}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11">
-        <v>150696</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6">
-        <v>43.31</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDA93F7-147E-4836-8A7C-A6951315924A}">
   <dimension ref="A1:L2"/>
   <sheetViews>

</xml_diff>